<commit_message>
Added one more scenario for authentication
</commit_message>
<xml_diff>
--- a/src/test/resources/testcase.xlsx
+++ b/src/test/resources/testcase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
   <si>
     <t>Execution</t>
   </si>
@@ -84,9 +84,6 @@
     <t>H22J38BABC</t>
   </si>
   <si>
-    <t>No Such Catalog in the site</t>
-  </si>
-  <si>
     <t>Product Comparision from Listing Page with  disabled Cart</t>
   </si>
   <si>
@@ -129,7 +126,19 @@
     <t>Verify when no such product exists</t>
   </si>
   <si>
-    <t xml:space="preserve">No Execution </t>
+    <t>InvalidPassword</t>
+  </si>
+  <si>
+    <t>TC_5</t>
+  </si>
+  <si>
+    <t>Verify when No Such Catalog in the site</t>
+  </si>
+  <si>
+    <t>Verify when Execution is set as N</t>
+  </si>
+  <si>
+    <t>Verify Authentication</t>
   </si>
 </sst>
 </file>
@@ -479,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -537,10 +546,10 @@
     </row>
     <row r="2" spans="1:12" ht="45">
       <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -575,16 +584,16 @@
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
@@ -602,27 +611,27 @@
         <v>17</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" t="s">
         <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -640,7 +649,7 @@
         <v>17</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>19</v>
@@ -651,16 +660,16 @@
     </row>
     <row r="5" spans="1:12" ht="45">
       <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>16</v>
@@ -678,24 +687,63 @@
         <v>17</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="E5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>